<commit_message>
synthesis increment and skip adders
</commit_message>
<xml_diff>
--- a/Sythesis/Dataadders.xlsx
+++ b/Sythesis/Dataadders.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmed sabry\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Engineering\Third_Year\CMP_2023\First_Term\VLSI\Project\Project\VLSI\Sythesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A109ED81-15E3-47D1-AE53-B00C0607E059}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03C3716D-FFC7-4018-8416-E56A8AB5F19C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11412" yWindow="1500" windowWidth="11520" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -404,8 +404,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:L10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -585,25 +585,87 @@
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="1"/>
+      <c r="B7" s="1">
+        <v>500</v>
+      </c>
+      <c r="C7">
+        <v>15635.7</v>
+      </c>
+      <c r="F7">
+        <v>3864.3</v>
+      </c>
+      <c r="G7">
+        <v>42</v>
+      </c>
+      <c r="H7">
+        <v>149</v>
+      </c>
+      <c r="I7">
+        <v>9.0061979999999995</v>
+      </c>
+      <c r="J7">
+        <v>2.7300589999999998</v>
+      </c>
+      <c r="K7">
+        <v>18.160315000000001</v>
+      </c>
+      <c r="L7">
+        <v>20</v>
+      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="1"/>
+      <c r="B8" s="1">
+        <v>500</v>
+      </c>
+      <c r="C8">
+        <v>16551.400000000001</v>
+      </c>
+      <c r="F8">
+        <v>2948.6</v>
+      </c>
+      <c r="G8">
+        <v>69</v>
+      </c>
+      <c r="H8">
+        <v>183</v>
+      </c>
+      <c r="I8">
+        <v>10.459711</v>
+      </c>
+      <c r="J8">
+        <v>3.5181369999999998</v>
+      </c>
+      <c r="K8">
+        <v>21.750378000000001</v>
+      </c>
+      <c r="L8">
+        <v>20</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="1"/>
+      <c r="B9" s="1">
+        <v>500</v>
+      </c>
+      <c r="L9">
+        <v>20</v>
+      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="1"/>
+      <c r="B10" s="1">
+        <v>500</v>
+      </c>
+      <c r="L10">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
synthesis carry select and bypass adders
</commit_message>
<xml_diff>
--- a/Sythesis/Dataadders.xlsx
+++ b/Sythesis/Dataadders.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Engineering\Third_Year\CMP_2023\First_Term\VLSI\Project\Project\VLSI\Sythesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03C3716D-FFC7-4018-8416-E56A8AB5F19C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BF72051-F9F4-42CC-A125-7985FE5F709B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11412" yWindow="1500" windowWidth="11520" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -405,7 +405,7 @@
   <dimension ref="A2:L10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -652,6 +652,27 @@
       <c r="B9" s="1">
         <v>500</v>
       </c>
+      <c r="C9">
+        <v>15276.3</v>
+      </c>
+      <c r="F9">
+        <v>4223.7</v>
+      </c>
+      <c r="G9">
+        <v>78</v>
+      </c>
+      <c r="H9">
+        <v>207</v>
+      </c>
+      <c r="I9">
+        <v>10.944514</v>
+      </c>
+      <c r="J9">
+        <v>4.015822</v>
+      </c>
+      <c r="K9">
+        <v>23.751881000000001</v>
+      </c>
       <c r="L9">
         <v>20</v>
       </c>
@@ -662,6 +683,27 @@
       </c>
       <c r="B10" s="1">
         <v>500</v>
+      </c>
+      <c r="C10">
+        <v>15613.1</v>
+      </c>
+      <c r="F10">
+        <v>3886.9</v>
+      </c>
+      <c r="G10">
+        <v>68</v>
+      </c>
+      <c r="H10">
+        <v>238</v>
+      </c>
+      <c r="I10">
+        <v>10.567257</v>
+      </c>
+      <c r="J10">
+        <v>4.3081699999999996</v>
+      </c>
+      <c r="K10">
+        <v>25.079926</v>
       </c>
       <c r="L10">
         <v>20</v>

</xml_diff>

<commit_message>
update synthesis of adders
</commit_message>
<xml_diff>
--- a/Sythesis/Dataadders.xlsx
+++ b/Sythesis/Dataadders.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Engineering\Third_Year\CMP_2023\First_Term\VLSI\Project\Project\VLSI\Sythesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88225650-D08E-4D34-8456-A43EFC3C1798}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{428807F4-FF7B-4BB6-8848-A661037A5890}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11412" yWindow="1500" windowWidth="11520" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -404,13 +404,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:L10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="21.33203125" customWidth="1"/>
+    <col min="1" max="1" width="21.33203125" customWidth="1"/>
+    <col min="2" max="2" width="21.33203125" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="12.5546875" customWidth="1"/>
     <col min="4" max="4" width="13.6640625" customWidth="1"/>
     <col min="5" max="5" width="15.77734375" customWidth="1"/>
@@ -525,10 +526,10 @@
         <v>500</v>
       </c>
       <c r="C5">
-        <v>16414.3</v>
+        <v>16560.400000000001</v>
       </c>
       <c r="F5">
-        <v>3085.7</v>
+        <v>2939.6</v>
       </c>
       <c r="G5">
         <v>124</v>
@@ -589,10 +590,10 @@
         <v>500</v>
       </c>
       <c r="C7">
-        <v>15635.7</v>
+        <v>16609.099999999999</v>
       </c>
       <c r="F7">
-        <v>3864.3</v>
+        <v>2890.9</v>
       </c>
       <c r="G7">
         <v>42</v>
@@ -621,10 +622,10 @@
         <v>500</v>
       </c>
       <c r="C8">
-        <v>16551.400000000001</v>
+        <v>17020.3</v>
       </c>
       <c r="F8">
-        <v>2948.6</v>
+        <v>2479.6999999999998</v>
       </c>
       <c r="G8">
         <v>69</v>
@@ -653,10 +654,10 @@
         <v>500</v>
       </c>
       <c r="C9">
-        <v>15276.3</v>
+        <v>15585.5</v>
       </c>
       <c r="F9">
-        <v>4223.7</v>
+        <v>3914.5</v>
       </c>
       <c r="G9">
         <v>78</v>
@@ -685,25 +686,25 @@
         <v>500</v>
       </c>
       <c r="C10">
-        <v>15613.1</v>
+        <v>17399.400000000001</v>
       </c>
       <c r="F10">
-        <v>3886.9</v>
+        <v>2100.6</v>
       </c>
       <c r="G10">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H10">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="I10">
-        <v>10.567257</v>
+        <v>11.118458</v>
       </c>
       <c r="J10">
-        <v>4.3081699999999996</v>
+        <v>4.3387460000000004</v>
       </c>
       <c r="K10">
-        <v>25.079926</v>
+        <v>25.687866</v>
       </c>
       <c r="L10">
         <v>20</v>

</xml_diff>